<commit_message>
Update document content and CSV files; delete obsolete PDF files and implement input dialog functionality
</commit_message>
<xml_diff>
--- a/Temp/temp1.xlsx
+++ b/Temp/temp1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Infrastructure Type</t>
   </si>
@@ -61,7 +61,7 @@
     <t>asd</t>
   </si>
   <si>
-    <t>king</t>
+    <t>da</t>
   </si>
   <si>
     <t>dsaf</t>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Accepted</t>
+  </si>
+  <si>
+    <t>Minor Deficiencies</t>
   </si>
 </sst>
 </file>
@@ -144,7 +147,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -163,6 +166,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -557,7 +567,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -577,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
@@ -594,9 +604,12 @@
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Removed">
       <formula>NOT(ISERROR(SEARCH("Removed",A1)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Minor Deficiencies">
+      <formula>NOT(ISERROR(SEARCH("Minor Deficiencies",A1)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I5">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update document templates: modify layout and formatting in test_copy.docx and adjust structure in asset list PDF for improved clarity and consistency
</commit_message>
<xml_diff>
--- a/Temp/temp1.xlsx
+++ b/Temp/temp1.xlsx
@@ -14,72 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
-  <si>
-    <t>Infrastructure Type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>Subarea</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Structure</t>
+    <t>Approved CCTV Vendor</t>
   </si>
   <si>
     <t>Warranty</t>
   </si>
   <si>
+    <t>OC Surveyor</t>
+  </si>
+  <si>
+    <t>Reviewer.1</t>
+  </si>
+  <si>
     <t>Notes.1</t>
   </si>
   <si>
-    <t>Mechanical</t>
-  </si>
-  <si>
-    <t>Electrical</t>
-  </si>
-  <si>
-    <t>Health and Safety</t>
-  </si>
-  <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t>dsf</t>
-  </si>
-  <si>
-    <t>asdsa</t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>dsa</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>da</t>
-  </si>
-  <si>
-    <t>dsaf</t>
-  </si>
-  <si>
-    <t>ads</t>
-  </si>
-  <si>
-    <t>das</t>
+    <t>gh</t>
+  </si>
+  <si>
+    <t>GPH</t>
   </si>
   <si>
     <t>Accepted</t>
   </si>
   <si>
-    <t>Minor Deficiencies</t>
-  </si>
-  <si>
-    <t>sads</t>
+    <t>COSTELLO_C</t>
+  </si>
+  <si>
+    <t>T. Martin</t>
+  </si>
+  <si>
+    <t>hg</t>
   </si>
 </sst>
 </file>
@@ -484,17 +457,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="1" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,97 +486,34 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="H2" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +531,7 @@
       <formula>NOT(ISERROR(SEARCH("Minor Deficiencies",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:I5">
+  <conditionalFormatting sqref="B2:L2">
     <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>